<commit_message>
Updated with 1c task as completed And started with 2a
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
+++ b/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git-Repository\PRY-CC\docs\bio metric integration estimation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="21975" windowHeight="15240"/>
+    <workbookView xWindow="120" yWindow="20" windowWidth="24900" windowHeight="17100"/>
   </bookViews>
   <sheets>
     <sheet name="iOS_Estimate" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Functionality</t>
   </si>
@@ -541,26 +536,26 @@
   <dimension ref="A2:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="81" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="20">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="20">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,7 +581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="7"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -596,7 +591,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="7"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -606,7 +601,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
@@ -618,7 +613,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
@@ -640,7 +635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
@@ -664,7 +659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -685,10 +680,10 @@
         <v>42213</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="10"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -698,7 +693,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
@@ -710,7 +705,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
@@ -722,11 +717,17 @@
       <c r="E13" s="4">
         <v>4</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="15">
+        <v>42214</v>
+      </c>
+      <c r="G13" s="15">
+        <v>42214</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -746,7 +747,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -764,7 +765,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="12"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -774,7 +775,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="8" t="s">
         <v>8</v>
       </c>
@@ -788,7 +789,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="12" t="s">
         <v>13</v>
       </c>
@@ -806,7 +807,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
@@ -822,7 +823,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="10"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -832,7 +833,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
@@ -846,7 +847,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="14" t="s">
         <v>18</v>
       </c>
@@ -864,7 +865,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="10" t="s">
         <v>17</v>
       </c>
@@ -880,7 +881,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="10"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -890,7 +891,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="8" t="s">
         <v>11</v>
       </c>
@@ -904,7 +905,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
@@ -922,7 +923,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
         <v>22</v>
       </c>
@@ -938,7 +939,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="8"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -948,7 +949,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="8" t="s">
         <v>12</v>
       </c>
@@ -962,7 +963,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="13" t="s">
         <v>18</v>
       </c>
@@ -980,7 +981,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="8" t="s">
         <v>17</v>
       </c>
@@ -996,7 +997,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="8"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1006,7 +1007,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="8" t="s">
         <v>24</v>
       </c>
@@ -1018,7 +1019,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1028,7 +1029,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1038,7 +1039,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1057,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1066,7 +1067,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1076,7 +1077,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1086,7 +1087,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1096,7 +1097,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1123,7 +1124,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1140,7 +1141,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Completed 2a and 7a points
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
+++ b/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Functionality</t>
   </si>
@@ -116,7 +116,7 @@
     <t>completed</t>
   </si>
   <si>
-    <t>in progress</t>
+    <t>a.created ipa to determine parameters of wifi</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -231,6 +231,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +539,7 @@
   <dimension ref="A2:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -724,7 +727,7 @@
         <v>42214</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1020,11 +1023,17 @@
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="4">
+        <v>3</v>
+      </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4">
+        <v>3</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -1044,14 +1053,14 @@
         <v>3</v>
       </c>
       <c r="B36" s="4">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C36" s="4">
         <v>14</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="6">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>

</xml_diff>

<commit_message>
Started with 3a and 3b
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
+++ b/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Functionality</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>a.created ipa to determine parameters of wifi</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
   <dimension ref="A2:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -806,9 +809,13 @@
       <c r="E18" s="4">
         <v>7</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="15">
+        <v>42215</v>
+      </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="10" t="s">
@@ -822,9 +829,13 @@
       <c r="E19" s="4">
         <v>3</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="15">
+        <v>42215</v>
+      </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="10"/>
@@ -1034,9 +1045,15 @@
       <c r="E34" s="4">
         <v>3</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="F34" s="15">
+        <v>42215</v>
+      </c>
+      <c r="G34" s="15">
+        <v>42215</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="4"/>

</xml_diff>

<commit_message>
Completed Quality Check iOS Part
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
+++ b/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="30620" windowHeight="17160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28160" windowHeight="17000"/>
   </bookViews>
   <sheets>
     <sheet name="iOS_Estimate" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Functionality</t>
   </si>
@@ -116,16 +116,38 @@
     <t>completed</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>a.Created ipa file for determining wifi params</t>
   </si>
   <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Completed Development.Facing "the requested resource does not support http method 'post'. error".Need input from biometric Team.</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Webservice from Hybris Team</t>
+  </si>
+  <si>
+    <t>Need Webervice from Swarnima to proceed.</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Completed Development.Facing "the requested resource does not support http method 'post'. error".Need input from biometric Team. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solved the issue with Pavan's Input on 3rd Aug</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -553,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -597,7 +619,7 @@
         <v>28</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>29</v>
@@ -769,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -824,7 +846,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="56">
+    <row r="18" spans="1:9" ht="70">
       <c r="A18" s="12" t="s">
         <v>13</v>
       </c>
@@ -841,12 +863,14 @@
       <c r="F18" s="15">
         <v>42215</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="15">
+        <v>42219</v>
+      </c>
       <c r="H18" s="19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -864,10 +888,12 @@
       <c r="F19" s="15">
         <v>42216</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="15">
+        <v>42219</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -888,7 +914,7 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -950,7 +976,7 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1012,7 +1038,7 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1034,10 +1060,16 @@
       <c r="E30" s="4">
         <v>6</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="15">
+        <v>42220</v>
+      </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="8" t="s">
@@ -1051,10 +1083,14 @@
       <c r="E31" s="4">
         <v>2</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="15">
+        <v>42220</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="8"/>
@@ -1082,7 +1118,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4">
         <v>4</v>

</xml_diff>

<commit_message>
Updated Status on getting Threshold of Image
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
+++ b/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Functionality</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>6.Getting the details of parameters from WIFI network connected to iPhone.</t>
+  </si>
+  <si>
+    <t>Set up the hybris server and done initialisation to set up the code.Development Done.Not Getting response from hybris sever</t>
+  </si>
+  <si>
+    <t>Started Writing client code and methods.Waiting for updated webservice from Swarnima.</t>
   </si>
 </sst>
 </file>
@@ -570,7 +576,7 @@
   <dimension ref="A2:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -774,7 +780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="42">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -790,10 +796,16 @@
       <c r="E14" s="4">
         <v>5</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="14">
+        <v>42222</v>
+      </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="H14" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
@@ -1003,7 +1015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="42">
       <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1019,7 +1031,9 @@
         <v>42220</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="I27" s="4" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updated iOS Tasks Status.
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
+++ b/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Functionality</t>
   </si>
@@ -147,10 +147,26 @@
     <t>6.Getting the details of parameters from WIFI network connected to iPhone.</t>
   </si>
   <si>
-    <t>Set up the hybris server and done initialisation to set up the code.Development Done.Not Getting response from hybris sever</t>
-  </si>
-  <si>
-    <t>Started Writing client code and methods.Waiting for updated webservice from Swarnima.</t>
+    <r>
+      <t>Set up the hybris server and done initialisation to set up the code.Development Done.Not Getting response from hybris sever.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Got the Successful response on 7th Aug.</t>
+    </r>
+  </si>
+  <si>
+    <t>Started Writing client code and methods.Waiting for updated webservice from Swarnima.Development Done.Getting 200 OK but not getting desired response i.e. ProfilepicURL.</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -576,7 +592,7 @@
   <dimension ref="A2:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -780,7 +796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="42">
+    <row r="14" spans="1:9" ht="70">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -824,7 +840,9 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="12"/>
@@ -942,10 +960,16 @@
       <c r="E22" s="4">
         <v>7</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="14">
+        <v>42226</v>
+      </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="8" t="s">
@@ -959,10 +983,14 @@
       <c r="E23" s="4">
         <v>3</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="14">
+        <v>42226</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="8"/>
@@ -1007,15 +1035,17 @@
       <c r="F26" s="14">
         <v>42220</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="14">
+        <v>42223</v>
+      </c>
       <c r="H26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="42">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="56">
       <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1030,12 +1060,14 @@
       <c r="F27" s="14">
         <v>42220</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="14">
+        <v>42223</v>
+      </c>
       <c r="H27" s="18" t="s">
         <v>37</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:9">

</xml_diff>

<commit_message>
Updated Status of FB & instagram Integration
</commit_message>
<xml_diff>
--- a/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
+++ b/docs/bio metric integration estimation/MDI_iOSDevelopment_Timelines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="iOS_Estimate" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Functionality</t>
   </si>
@@ -32,9 +32,6 @@
     <t>TOTAL(hours)</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>1. Capture the image from front or back camera of iphone.</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>b.Call Webservice for getting url for profile pic.</t>
   </si>
   <si>
-    <t xml:space="preserve">c.create local db /Directory to save the profile pic  </t>
-  </si>
-  <si>
     <t>3. Webservice implementation for Verify the quality of the image captured from iphone .</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
   </si>
   <si>
     <t>Need Webervice from Swarnima to proceed.</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <r>
@@ -161,12 +152,6 @@
       </rPr>
       <t xml:space="preserve"> Got the Successful response on 7th Aug.</t>
     </r>
-  </si>
-  <si>
-    <t>Waiting for the Profile Url to save in local Db.</t>
-  </si>
-  <si>
-    <t>Started Writing client code and methods.Development Done.Getting 200 OK but not getting desired response i.e. ProfilepicURL.</t>
   </si>
   <si>
     <r>
@@ -204,12 +189,47 @@
       <t>Got the Successful response on 19 Aug.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>Started Writing client code and methods.Development Done.Getting 200 OK but not getting desired response i.e. ProfilepicURL.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Got the Successful response on 27 Aug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>7. Instagram Integration to import profile picture.</t>
+  </si>
+  <si>
+    <t>8.Facebook integration to import profile picture</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +258,22 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -279,8 +315,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -331,7 +369,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -632,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I37"/>
+  <dimension ref="A2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -660,28 +700,28 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -708,7 +748,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -721,7 +761,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -739,12 +779,12 @@
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4">
         <v>6</v>
@@ -764,12 +804,12 @@
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4">
         <v>6</v>
@@ -789,7 +829,7 @@
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -805,7 +845,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -818,7 +858,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4">
         <v>4</v>
@@ -836,12 +876,12 @@
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="56">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="70">
       <c r="A14" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="4">
         <v>4</v>
@@ -850,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
@@ -858,36 +898,26 @@
       <c r="F14" s="14">
         <v>42222</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="14">
+        <v>42243</v>
+      </c>
       <c r="H14" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
+      <c r="A15" s="12"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4">
-        <v>7</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="12"/>
@@ -902,12 +932,12 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -917,7 +947,7 @@
     </row>
     <row r="18" spans="1:9" ht="70">
       <c r="A18" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" s="4">
         <v>5</v>
@@ -936,15 +966,15 @@
         <v>42219</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" s="4">
         <v>3</v>
@@ -962,7 +992,7 @@
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -978,12 +1008,12 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -993,7 +1023,7 @@
     </row>
     <row r="22" spans="1:9" ht="84">
       <c r="A22" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4">
         <v>5</v>
@@ -1010,15 +1040,15 @@
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>
@@ -1034,7 +1064,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1050,12 +1080,12 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1065,7 +1095,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26" s="4">
         <v>4</v>
@@ -1084,15 +1114,15 @@
         <v>42223</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="70">
       <c r="A27" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27" s="4">
         <v>2</v>
@@ -1109,10 +1139,10 @@
         <v>42223</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1128,7 +1158,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1141,7 +1171,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B30" s="4">
         <v>4</v>
@@ -1159,60 +1189,80 @@
       </c>
       <c r="H30" s="14"/>
       <c r="I30" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="4"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="5" t="s">
-        <v>3</v>
+      <c r="A32" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B32" s="4">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C32" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="6">
-        <v>66</v>
-      </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="E32" s="4">
+        <v>10</v>
+      </c>
+      <c r="F32" s="14">
+        <v>42242</v>
+      </c>
+      <c r="G32" s="14">
+        <v>42244</v>
+      </c>
       <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="4"/>
+      <c r="A33" s="5"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="6"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="A34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="4">
+        <v>8</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2</v>
+      </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="E34" s="4">
+        <v>10</v>
+      </c>
+      <c r="F34" s="14">
+        <v>42241</v>
+      </c>
+      <c r="G34" s="14">
+        <v>42242</v>
+      </c>
       <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="4"/>
@@ -1226,12 +1276,20 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="A36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="5">
+        <v>64</v>
+      </c>
+      <c r="C36" s="5">
+        <v>15</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5">
+        <v>79</v>
+      </c>
+      <c r="F36" s="5"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -1246,6 +1304,17 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>